<commit_message>
combine the name with same substring
</commit_message>
<xml_diff>
--- a/UniversityLocation.xlsx
+++ b/UniversityLocation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xuhao.du.UWA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xuhao.du.UWA\Peter Du\University entrance exam\Chinese_University_Entrance_Ranking_GD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1588"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1462" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A1462" sqref="A1462"/>
+    <sheetView tabSelected="1" topLeftCell="A1560" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1584" sqref="B1584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="449" spans="1:2">
       <c r="A449" s="1" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B449" s="1" t="s">
         <v>166</v>

</xml_diff>